<commit_message>
Update analyses 010 and 013
Add extra pathway to heatmap and make special row names for heatmap
</commit_message>
<xml_diff>
--- a/data/cleaned/013_pathways.xlsx
+++ b/data/cleaned/013_pathways.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jegoussc/GitHub/PD_PRO_1499_06122021_PRM2/cleaned/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jegoussc/GitHub/PD_PRO_1499_06122021_PRM2/data/cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BFCA1F-9177-4F47-9BD1-67E5BECAF42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119CC327-497B-CC41-A758-09677BFFDD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="820" windowWidth="27640" windowHeight="15940" xr2:uid="{44844078-B70E-D04A-B184-47806E995AF4}"/>
+    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16240" xr2:uid="{44844078-B70E-D04A-B184-47806E995AF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Early appressorium pathways" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="256">
   <si>
     <t>Pth11</t>
   </si>
@@ -582,6 +582,228 @@
   </si>
   <si>
     <t>Autophagy</t>
+  </si>
+  <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>TOR1</t>
+  </si>
+  <si>
+    <t>LST8</t>
+  </si>
+  <si>
+    <t>MGG_07284</t>
+  </si>
+  <si>
+    <t>MIP1</t>
+  </si>
+  <si>
+    <t>MGG_02874</t>
+  </si>
+  <si>
+    <t>BIT61</t>
+  </si>
+  <si>
+    <t>MGG_11443</t>
+  </si>
+  <si>
+    <t>MAPKAP1</t>
+  </si>
+  <si>
+    <t>MGG_12955</t>
+  </si>
+  <si>
+    <t>spherulin-1b precursor</t>
+  </si>
+  <si>
+    <t>MGG_15259</t>
+  </si>
+  <si>
+    <t>TSC11</t>
+  </si>
+  <si>
+    <t>MGG_05284</t>
+  </si>
+  <si>
+    <t>IML1</t>
+  </si>
+  <si>
+    <t>MGG_04160</t>
+  </si>
+  <si>
+    <t>SCH9</t>
+  </si>
+  <si>
+    <t>MGG_14773</t>
+  </si>
+  <si>
+    <t>tor signaling pathway regulator</t>
+  </si>
+  <si>
+    <t>MGG_01540</t>
+  </si>
+  <si>
+    <t>RPS6</t>
+  </si>
+  <si>
+    <t>YPK1</t>
+  </si>
+  <si>
+    <t>ORM1</t>
+  </si>
+  <si>
+    <t>MGG_16259</t>
+  </si>
+  <si>
+    <t>LCB1</t>
+  </si>
+  <si>
+    <t>MGG_00864</t>
+  </si>
+  <si>
+    <t>LCB2</t>
+  </si>
+  <si>
+    <t>MGG_05197</t>
+  </si>
+  <si>
+    <t>phosphoinositide phosphatase</t>
+  </si>
+  <si>
+    <t>MGG_11279</t>
+  </si>
+  <si>
+    <t>PP2a</t>
+  </si>
+  <si>
+    <t>MGG_05637</t>
+  </si>
+  <si>
+    <t>LAC1</t>
+  </si>
+  <si>
+    <t>MGG_05189</t>
+  </si>
+  <si>
+    <t>LAG1</t>
+  </si>
+  <si>
+    <t>MGG_03090</t>
+  </si>
+  <si>
+    <t>ELO1</t>
+  </si>
+  <si>
+    <t>MGG_07280</t>
+  </si>
+  <si>
+    <t>FPK1</t>
+  </si>
+  <si>
+    <t>MGG_07012</t>
+  </si>
+  <si>
+    <t>MgAPT2</t>
+  </si>
+  <si>
+    <t>MGG_02767</t>
+  </si>
+  <si>
+    <t>GIN4</t>
+  </si>
+  <si>
+    <t>MGG_02810</t>
+  </si>
+  <si>
+    <t>GPD1</t>
+  </si>
+  <si>
+    <t>MGG_00067</t>
+  </si>
+  <si>
+    <t>mip family channel protein</t>
+  </si>
+  <si>
+    <t>MGG_13615</t>
+  </si>
+  <si>
+    <t>ph domain-containing protein</t>
+  </si>
+  <si>
+    <t>MGG_03558</t>
+  </si>
+  <si>
+    <t>MGG_01047</t>
+  </si>
+  <si>
+    <t>PKC1</t>
+  </si>
+  <si>
+    <t>RHO1</t>
+  </si>
+  <si>
+    <t>MGG_07176</t>
+  </si>
+  <si>
+    <t>rho1 guanine nucleotide exchange factor 1</t>
+  </si>
+  <si>
+    <t>MGG_03064</t>
+  </si>
+  <si>
+    <t>MPS1</t>
+  </si>
+  <si>
+    <t>MGG_04943</t>
+  </si>
+  <si>
+    <t>KSG1</t>
+  </si>
+  <si>
+    <t>MGG_01795</t>
+  </si>
+  <si>
+    <t>CPKA</t>
+  </si>
+  <si>
+    <t>EHS1</t>
+  </si>
+  <si>
+    <t>MGG_12128</t>
+  </si>
+  <si>
+    <t>CMKK2/MoTos3</t>
+  </si>
+  <si>
+    <t>MGG_06421</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>wdA (AN1056)</t>
+  </si>
+  <si>
+    <t>MGG_06968</t>
+  </si>
+  <si>
+    <t>mcnC/Def1 (AN2871)</t>
+  </si>
+  <si>
+    <t>MGG_00124</t>
+  </si>
+  <si>
+    <t>Tubulin binding Cofactor A (TBCA)  (AN6176)</t>
+  </si>
+  <si>
+    <t>MGG_09890</t>
+  </si>
+  <si>
+    <t> Elongation Factor 2 (AN6330)</t>
+  </si>
+  <si>
+    <t>MGG_01742</t>
   </si>
 </sst>
 </file>
@@ -955,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D602909-41E2-0A47-9956-63737B5EBCFB}">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70:A92"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1979,6 +2201,435 @@
         <v>169</v>
       </c>
     </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B93" t="s">
+        <v>183</v>
+      </c>
+      <c r="C93" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B94" t="s">
+        <v>184</v>
+      </c>
+      <c r="C94" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B95" t="s">
+        <v>186</v>
+      </c>
+      <c r="C95" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B96" t="s">
+        <v>188</v>
+      </c>
+      <c r="C96" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B97" t="s">
+        <v>190</v>
+      </c>
+      <c r="C97" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B98" t="s">
+        <v>192</v>
+      </c>
+      <c r="C98" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B99" t="s">
+        <v>194</v>
+      </c>
+      <c r="C99" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B100" t="s">
+        <v>196</v>
+      </c>
+      <c r="C100" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B101" t="s">
+        <v>198</v>
+      </c>
+      <c r="C101" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B102" t="s">
+        <v>200</v>
+      </c>
+      <c r="C102" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B103" t="s">
+        <v>202</v>
+      </c>
+      <c r="C103" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B104" t="s">
+        <v>203</v>
+      </c>
+      <c r="C104" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B105" t="s">
+        <v>204</v>
+      </c>
+      <c r="C105" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B106" t="s">
+        <v>206</v>
+      </c>
+      <c r="C106" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B107" t="s">
+        <v>208</v>
+      </c>
+      <c r="C107" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B108" t="s">
+        <v>210</v>
+      </c>
+      <c r="C108" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B109" t="s">
+        <v>212</v>
+      </c>
+      <c r="C109" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B110" t="s">
+        <v>214</v>
+      </c>
+      <c r="C110" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B111" t="s">
+        <v>216</v>
+      </c>
+      <c r="C111" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B112" t="s">
+        <v>218</v>
+      </c>
+      <c r="C112" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B113" t="s">
+        <v>220</v>
+      </c>
+      <c r="C113" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B114" t="s">
+        <v>222</v>
+      </c>
+      <c r="C114" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B115" t="s">
+        <v>224</v>
+      </c>
+      <c r="C115" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B116" t="s">
+        <v>226</v>
+      </c>
+      <c r="C116" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B117" t="s">
+        <v>228</v>
+      </c>
+      <c r="C117" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B118" t="s">
+        <v>230</v>
+      </c>
+      <c r="C118" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B119" t="s">
+        <v>230</v>
+      </c>
+      <c r="C119" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B120" t="s">
+        <v>233</v>
+      </c>
+      <c r="C120" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B121" t="s">
+        <v>234</v>
+      </c>
+      <c r="C121" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B122" t="s">
+        <v>236</v>
+      </c>
+      <c r="C122" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B123" t="s">
+        <v>238</v>
+      </c>
+      <c r="C123" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B124" t="s">
+        <v>240</v>
+      </c>
+      <c r="C124" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B125" t="s">
+        <v>242</v>
+      </c>
+      <c r="C125" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B126" t="s">
+        <v>243</v>
+      </c>
+      <c r="C126" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B127" t="s">
+        <v>245</v>
+      </c>
+      <c r="C127" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B128" t="s">
+        <v>248</v>
+      </c>
+      <c r="C128" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B129" t="s">
+        <v>250</v>
+      </c>
+      <c r="C129" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B130" t="s">
+        <v>252</v>
+      </c>
+      <c r="C130" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B131" t="s">
+        <v>254</v>
+      </c>
+      <c r="C131" t="s">
+        <v>255</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>